<commit_message>
corrected values in umsatz_ergebnis.csv and .xlsx
</commit_message>
<xml_diff>
--- a/data/umsatz_ergebnis.xlsx
+++ b/data/umsatz_ergebnis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conny\Desktop\Computerlinguistik\Semester 8\Tabellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FAE04F-969C-47C9-A921-7FE4E678B0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44D31FE-8E36-42C6-97C7-46A502D3056F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2F68C51D-CCC7-44E3-A77B-79C4056E9987}"/>
+    <workbookView xWindow="3276" yWindow="3276" windowWidth="17280" windowHeight="8880" xr2:uid="{2F68C51D-CCC7-44E3-A77B-79C4056E9987}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,13 +630,13 @@
         <v>35844000000</v>
       </c>
       <c r="C10">
-        <v>2810335844000000</v>
+        <v>28103000000</v>
       </c>
       <c r="D10">
-        <v>297435844000000</v>
+        <v>2974000000</v>
       </c>
       <c r="E10">
-        <v>216335844000000</v>
+        <v>2163000000</v>
       </c>
       <c r="F10">
         <v>2018</v>

</xml_diff>